<commit_message>
Updated summary of alternative forecast values/ranges
</commit_message>
<xml_diff>
--- a/figs/Cunningham Kusko Forecast Summary.xlsx
+++ b/figs/Cunningham Kusko Forecast Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/curryc2/Documents/2020/AYK/Kuskokwim Consulting/Kuskokwim-Chinook-Preseason-Forecast/figs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{83448687-A4BE-A241-AF0B-A7ECE48D3DB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38319BA-2CBE-3D46-BC2F-3FB477AC1243}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39080" yWindow="1140" windowWidth="27640" windowHeight="16940" xr2:uid="{A5CFC254-5DA8-D849-8312-1C3B5A59A770}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21180" xr2:uid="{A5CFC254-5DA8-D849-8312-1C3B5A59A770}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="8">
   <si>
     <t>AR1-Empirical</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>CV</t>
+  </si>
+  <si>
+    <t>Lower 95% HDI</t>
+  </si>
+  <si>
+    <t>Upper 95% HDI</t>
+  </si>
+  <si>
+    <t>Model</t>
   </si>
 </sst>
 </file>
@@ -95,11 +104,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -415,14 +426,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4ACABC7-E291-B742-8393-DBF4874C3AE1}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C9"/>
+      <selection activeCell="A24" sqref="A24:K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -525,6 +537,255 @@
         <v>258642.84210630201</v>
       </c>
     </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4">
+        <v>110000</v>
+      </c>
+      <c r="C10" s="4">
+        <v>172000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4">
+        <v>328000</v>
+      </c>
+      <c r="C11" s="4">
+        <v>256000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F17">
+        <v>0.25</v>
+      </c>
+      <c r="G17">
+        <v>0.5</v>
+      </c>
+      <c r="H17">
+        <v>0.75</v>
+      </c>
+      <c r="I17">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="J17" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>213317.467815343</v>
+      </c>
+      <c r="C18">
+        <v>58060.452444853399</v>
+      </c>
+      <c r="D18">
+        <v>0.27217861265404242</v>
+      </c>
+      <c r="E18">
+        <v>121446.57067827</v>
+      </c>
+      <c r="F18">
+        <v>171732.38381670101</v>
+      </c>
+      <c r="G18">
+        <v>205943.77193442601</v>
+      </c>
+      <c r="H18">
+        <v>246675.25088838401</v>
+      </c>
+      <c r="I18">
+        <v>347561.76785331802</v>
+      </c>
+      <c r="J18">
+        <v>110000</v>
+      </c>
+      <c r="K18">
+        <v>328000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>213361.25441453099</v>
+      </c>
+      <c r="C19">
+        <v>21546.309475039401</v>
+      </c>
+      <c r="D19">
+        <v>0.10098510872633859</v>
+      </c>
+      <c r="E19">
+        <v>174124.38220897</v>
+      </c>
+      <c r="F19">
+        <v>198274.72760430499</v>
+      </c>
+      <c r="G19">
+        <v>212369.381770754</v>
+      </c>
+      <c r="H19">
+        <v>227248.057875008</v>
+      </c>
+      <c r="I19">
+        <v>258642.84210630201</v>
+      </c>
+      <c r="J19">
+        <v>172000</v>
+      </c>
+      <c r="K19">
+        <v>256000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F24">
+        <v>0.25</v>
+      </c>
+      <c r="G24">
+        <v>0.5</v>
+      </c>
+      <c r="H24">
+        <v>0.75</v>
+      </c>
+      <c r="I24">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="J24" t="s">
+        <v>5</v>
+      </c>
+      <c r="K24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="5">
+        <f>B18/1000</f>
+        <v>213.31746781534301</v>
+      </c>
+      <c r="C25" s="5">
+        <f t="shared" ref="C25:K26" si="0">C18/1000</f>
+        <v>58.060452444853397</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" si="0"/>
+        <v>2.7217861265404244E-4</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="0"/>
+        <v>121.44657067827001</v>
+      </c>
+      <c r="F25" s="5">
+        <f t="shared" si="0"/>
+        <v>171.732383816701</v>
+      </c>
+      <c r="G25" s="5">
+        <f t="shared" si="0"/>
+        <v>205.94377193442602</v>
+      </c>
+      <c r="H25" s="5">
+        <f t="shared" si="0"/>
+        <v>246.675250888384</v>
+      </c>
+      <c r="I25" s="5">
+        <f t="shared" si="0"/>
+        <v>347.56176785331803</v>
+      </c>
+      <c r="J25" s="5">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="K25" s="5">
+        <f t="shared" si="0"/>
+        <v>328</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="5">
+        <f>B19/1000</f>
+        <v>213.361254414531</v>
+      </c>
+      <c r="C26" s="5">
+        <f t="shared" si="0"/>
+        <v>21.546309475039401</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" si="0"/>
+        <v>1.0098510872633858E-4</v>
+      </c>
+      <c r="E26" s="5">
+        <f t="shared" si="0"/>
+        <v>174.12438220896999</v>
+      </c>
+      <c r="F26" s="5">
+        <f t="shared" si="0"/>
+        <v>198.27472760430499</v>
+      </c>
+      <c r="G26" s="5">
+        <f t="shared" si="0"/>
+        <v>212.36938177075399</v>
+      </c>
+      <c r="H26" s="5">
+        <f t="shared" si="0"/>
+        <v>227.24805787500802</v>
+      </c>
+      <c r="I26" s="5">
+        <f t="shared" si="0"/>
+        <v>258.642842106302</v>
+      </c>
+      <c r="J26" s="5">
+        <f t="shared" si="0"/>
+        <v>172</v>
+      </c>
+      <c r="K26" s="5">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>